<commit_message>
updating some classroom content for sprint 8
</commit_message>
<xml_diff>
--- a/Sprint00_Meta_Content/03_Useful_Snippets/Self Assessment Template.xlsx
+++ b/Sprint00_Meta_Content/03_Useful_Snippets/Self Assessment Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="24900" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="416">
   <si>
     <t>Data Journalist</t>
   </si>
@@ -1266,6 +1266,21 @@
   </si>
   <si>
     <t xml:space="preserve">Key </t>
+  </si>
+  <si>
+    <t>Random/Stochastic Processes and Variables</t>
+  </si>
+  <si>
+    <t>Applying Probability Models</t>
+  </si>
+  <si>
+    <t>update understanding with bayes</t>
+  </si>
+  <si>
+    <t>apply probability models</t>
+  </si>
+  <si>
+    <t>run monte carlo simulations</t>
   </si>
 </sst>
 </file>
@@ -1923,7 +1938,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2034,32 +2049,80 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2096,51 +2159,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2453,14 +2471,14 @@
       <c r="B1" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="54" t="s">
         <v>381</v>
       </c>
-      <c r="D1" s="81"/>
-      <c r="G1" s="80" t="s">
+      <c r="D1" s="54"/>
+      <c r="G1" s="53" t="s">
         <v>380</v>
       </c>
-      <c r="H1" s="80"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="29"/>
@@ -3497,10 +3515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3556,10 +3574,10 @@
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="55" t="s">
         <v>365</v>
       </c>
-      <c r="F5" s="83"/>
+      <c r="F5" s="56"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3632,10 +3650,10 @@
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
-      <c r="E11" s="84" t="s">
+      <c r="E11" s="57" t="s">
         <v>399</v>
       </c>
-      <c r="F11" s="85"/>
+      <c r="F11" s="58"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -3722,10 +3740,10 @@
       <c r="B18" s="33"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
-      <c r="E18" s="86" t="s">
+      <c r="E18" s="59" t="s">
         <v>400</v>
       </c>
-      <c r="F18" s="87"/>
+      <c r="F18" s="60"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
@@ -4020,16 +4038,16 @@
       <c r="D50" s="33"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>306</v>
-      </c>
-      <c r="B51" s="33"/>
-      <c r="C51" s="33"/>
-      <c r="D51" s="33"/>
+      <c r="A51" s="52" t="s">
+        <v>411</v>
+      </c>
+      <c r="B51" s="52"/>
+      <c r="C51" s="52"/>
+      <c r="D51" s="52"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
@@ -4037,7 +4055,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="33"/>
@@ -4045,7 +4063,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B54" s="33"/>
       <c r="C54" s="33"/>
@@ -4053,7 +4071,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B55" s="33"/>
       <c r="C55" s="33"/>
@@ -4061,7 +4079,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="33"/>
@@ -4069,7 +4087,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B57" s="33"/>
       <c r="C57" s="33"/>
@@ -4077,17 +4095,51 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B58" s="33"/>
       <c r="C58" s="33"/>
       <c r="D58" s="33"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="39"/>
-      <c r="B59" s="39"/>
-      <c r="C59" s="39"/>
-      <c r="D59" s="39"/>
+      <c r="A59" t="s">
+        <v>313</v>
+      </c>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="39" t="s">
+        <v>412</v>
+      </c>
+      <c r="B60" s="39"/>
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>413</v>
+      </c>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>414</v>
+      </c>
+      <c r="B62" s="33"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>415</v>
+      </c>
+      <c r="B63" s="33"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4103,7 +4155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
@@ -4119,10 +4171,10 @@
       <c r="B1" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="53" t="s">
         <v>410</v>
       </c>
-      <c r="E1" s="80"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
@@ -4512,8 +4564,8 @@
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="C17" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4527,64 +4579,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="63"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="66"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="82"/>
     </row>
     <row r="3" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="68"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
     </row>
     <row r="4" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
     </row>
     <row r="5" spans="1:6" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="87" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="72"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="88"/>
     </row>
     <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="73"/>
-      <c r="B6" s="74"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="73"/>
       <c r="C6" s="8" t="s">
         <v>34</v>
       </c>
@@ -4599,29 +4651,29 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52" t="s">
+      <c r="A7" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="57"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="68"/>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
-      <c r="B8" s="75" t="s">
+      <c r="A8" s="69"/>
+      <c r="B8" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="77"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="76"/>
     </row>
     <row r="9" spans="1:6" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
+      <c r="A9" s="69"/>
       <c r="B9" s="24" t="s">
         <v>49</v>
       </c>
@@ -4639,7 +4691,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="54"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="15" t="s">
         <v>50</v>
       </c>
@@ -4657,29 +4709,29 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="57"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
     </row>
     <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
-      <c r="B12" s="58" t="s">
+      <c r="A12" s="69"/>
+      <c r="B12" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="59"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="65"/>
     </row>
     <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
+      <c r="A13" s="69"/>
       <c r="B13" s="24" t="s">
         <v>51</v>
       </c>
@@ -4697,7 +4749,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
+      <c r="A14" s="69"/>
       <c r="B14" s="15" t="s">
         <v>52</v>
       </c>
@@ -4715,29 +4767,29 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="57"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="68"/>
     </row>
     <row r="16" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
-      <c r="B16" s="58" t="s">
+      <c r="A16" s="69"/>
+      <c r="B16" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="65"/>
     </row>
     <row r="17" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A17" s="53"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="24" t="s">
         <v>53</v>
       </c>
@@ -4755,7 +4807,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
+      <c r="A18" s="70"/>
       <c r="B18" s="15" t="s">
         <v>54</v>
       </c>
@@ -4773,29 +4825,29 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="57"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="53"/>
-      <c r="B20" s="58" t="s">
+      <c r="A20" s="69"/>
+      <c r="B20" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
     </row>
     <row r="21" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A21" s="53"/>
+      <c r="A21" s="69"/>
       <c r="B21" s="24" t="s">
         <v>55</v>
       </c>
@@ -4813,7 +4865,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
+      <c r="A22" s="69"/>
       <c r="B22" s="15" t="s">
         <v>56</v>
       </c>
@@ -4831,29 +4883,29 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="57"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="53"/>
-      <c r="B24" s="58" t="s">
+      <c r="A24" s="69"/>
+      <c r="B24" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="65"/>
     </row>
     <row r="25" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25" s="53"/>
+      <c r="A25" s="69"/>
       <c r="B25" s="24" t="s">
         <v>57</v>
       </c>
@@ -4871,7 +4923,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
+      <c r="A26" s="70"/>
       <c r="B26" s="15" t="s">
         <v>58</v>
       </c>
@@ -4889,29 +4941,29 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="68"/>
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="53"/>
-      <c r="B28" s="58" t="s">
+      <c r="A28" s="69"/>
+      <c r="B28" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="60"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="65"/>
     </row>
     <row r="29" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A29" s="53"/>
+      <c r="A29" s="69"/>
       <c r="B29" s="24" t="s">
         <v>59</v>
       </c>
@@ -4929,7 +4981,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
+      <c r="A30" s="69"/>
       <c r="B30" s="15" t="s">
         <v>60</v>
       </c>
@@ -4947,29 +4999,29 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="57"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="68"/>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="53"/>
-      <c r="B32" s="58" t="s">
+      <c r="A32" s="69"/>
+      <c r="B32" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="60"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="65"/>
     </row>
     <row r="33" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A33" s="53"/>
+      <c r="A33" s="69"/>
       <c r="B33" s="24" t="s">
         <v>74</v>
       </c>
@@ -4987,7 +5039,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="54"/>
+      <c r="A34" s="70"/>
       <c r="B34" s="15" t="s">
         <v>78</v>
       </c>
@@ -5005,29 +5057,29 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
-      <c r="F35" s="57"/>
+      <c r="C35" s="67"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="68"/>
     </row>
     <row r="36" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="53"/>
-      <c r="B36" s="58" t="s">
+      <c r="A36" s="69"/>
+      <c r="B36" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="60"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="65"/>
     </row>
     <row r="37" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A37" s="53"/>
+      <c r="A37" s="69"/>
       <c r="B37" s="24" t="s">
         <v>61</v>
       </c>
@@ -5045,7 +5097,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
+      <c r="A38" s="69"/>
       <c r="B38" s="15" t="s">
         <v>62</v>
       </c>
@@ -5063,29 +5115,29 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="68"/>
     </row>
     <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="53"/>
-      <c r="B40" s="58" t="s">
+      <c r="A40" s="69"/>
+      <c r="B40" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="59"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="60"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="65"/>
     </row>
     <row r="41" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="53"/>
+      <c r="A41" s="69"/>
       <c r="B41" s="24" t="s">
         <v>63</v>
       </c>
@@ -5103,7 +5155,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54"/>
+      <c r="A42" s="70"/>
       <c r="B42" s="15" t="s">
         <v>95</v>
       </c>
@@ -5121,29 +5173,29 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="55" t="s">
+      <c r="B43" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="56"/>
-      <c r="D43" s="56"/>
-      <c r="E43" s="56"/>
-      <c r="F43" s="57"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="68"/>
     </row>
     <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="53"/>
-      <c r="B44" s="58" t="s">
+      <c r="A44" s="69"/>
+      <c r="B44" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="60"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="65"/>
     </row>
     <row r="45" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A45" s="53"/>
+      <c r="A45" s="69"/>
       <c r="B45" s="24" t="s">
         <v>64</v>
       </c>
@@ -5161,7 +5213,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54"/>
+      <c r="A46" s="70"/>
       <c r="B46" s="15" t="s">
         <v>65</v>
       </c>
@@ -5179,8 +5231,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="78"/>
-      <c r="B47" s="79"/>
+      <c r="A47" s="61"/>
+      <c r="B47" s="62"/>
       <c r="C47" s="20" t="s">
         <v>0</v>
       </c>
@@ -5214,6 +5266,33 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B20:F20"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B36:F36"/>
@@ -5224,33 +5303,6 @@
     <mergeCell ref="B39:F39"/>
     <mergeCell ref="B44:F44"/>
     <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B20:F20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some sprint 8 updates
</commit_message>
<xml_diff>
--- a/Sprint00_Meta_Content/03_Useful_Snippets/Self Assessment Template.xlsx
+++ b/Sprint00_Meta_Content/03_Useful_Snippets/Self Assessment Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16800" windowHeight="18920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25720" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Concepts" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="474">
   <si>
     <t>Data Journalist</t>
   </si>
@@ -950,9 +950,6 @@
     <t>identify threats to validity</t>
   </si>
   <si>
-    <t>design objective and valid experiments</t>
-  </si>
-  <si>
     <t>simulate data for common probabiliy distribution</t>
   </si>
   <si>
@@ -1205,9 +1202,6 @@
     <t>Sampling , Instruments, and Bias</t>
   </si>
   <si>
-    <t xml:space="preserve">Implementing Tests </t>
-  </si>
-  <si>
     <t>Ive never heard of this before</t>
   </si>
   <si>
@@ -1268,12 +1262,6 @@
     <t xml:space="preserve">Key </t>
   </si>
   <si>
-    <t>Random/Stochastic Processes and Variables</t>
-  </si>
-  <si>
-    <t>Applying Probability Models</t>
-  </si>
-  <si>
     <t>update understanding with bayes</t>
   </si>
   <si>
@@ -1281,13 +1269,199 @@
   </si>
   <si>
     <t>run monte carlo simulations</t>
+  </si>
+  <si>
+    <t>Estimates, Hypotheses, Tests, Experiments</t>
+  </si>
+  <si>
+    <t>How do we estimate characteristics of the real world using data</t>
+  </si>
+  <si>
+    <t>How do we express the uncertainty in our estimates?</t>
+  </si>
+  <si>
+    <t>What are the different ways our estimate can be wrong?</t>
+  </si>
+  <si>
+    <t>How do we choose our estimates?</t>
+  </si>
+  <si>
+    <t>What kinds of models can we create from data?</t>
+  </si>
+  <si>
+    <t>How do we create models from the results of or experiments?</t>
+  </si>
+  <si>
+    <t>analyzing sampling performance</t>
+  </si>
+  <si>
+    <t>hypothesis testing</t>
+  </si>
+  <si>
+    <t>choosing a statistic</t>
+  </si>
+  <si>
+    <t>steps of statistical analysis</t>
+  </si>
+  <si>
+    <t>Probability Theory and Probability Models</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>effect size</t>
+  </si>
+  <si>
+    <t>probability mass function</t>
+  </si>
+  <si>
+    <t>percentile</t>
+  </si>
+  <si>
+    <t>probability density function</t>
+  </si>
+  <si>
+    <t>quantile</t>
+  </si>
+  <si>
+    <t>kernel density estimation</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>analytic distribution</t>
+  </si>
+  <si>
+    <t>binomial distribution</t>
+  </si>
+  <si>
+    <t>empirical distribution</t>
+  </si>
+  <si>
+    <t>multinomial distribution</t>
+  </si>
+  <si>
+    <t>standard normal distribution</t>
+  </si>
+  <si>
+    <t>poisson distribution</t>
+  </si>
+  <si>
+    <t>gaussian distribution</t>
+  </si>
+  <si>
+    <t>confidence interval</t>
+  </si>
+  <si>
+    <t>t-distribution</t>
+  </si>
+  <si>
+    <t>standard error</t>
+  </si>
+  <si>
+    <t>chi-square distribution</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>f-distribution</t>
+  </si>
+  <si>
+    <t>null hypothesis</t>
+  </si>
+  <si>
+    <t>bernoulli distribution</t>
+  </si>
+  <si>
+    <t>alternative hypothesis</t>
+  </si>
+  <si>
+    <t>independent vs dependent events</t>
+  </si>
+  <si>
+    <t>estimation</t>
+  </si>
+  <si>
+    <t>trials</t>
+  </si>
+  <si>
+    <t>estimator</t>
+  </si>
+  <si>
+    <t>outcomes</t>
+  </si>
+  <si>
+    <t>mean squared error</t>
+  </si>
+  <si>
+    <t>sample space</t>
+  </si>
+  <si>
+    <t>maximum likelood estimator</t>
+  </si>
+  <si>
+    <t>random variable</t>
+  </si>
+  <si>
+    <t>union</t>
+  </si>
+  <si>
+    <t>false positive, false negative</t>
+  </si>
+  <si>
+    <t>intersection</t>
+  </si>
+  <si>
+    <t>type1 / type 2 error</t>
+  </si>
+  <si>
+    <t>complement</t>
+  </si>
+  <si>
+    <t>internal / external validity</t>
+  </si>
+  <si>
+    <t>conditional probabiliy</t>
+  </si>
+  <si>
+    <t>threats to validity</t>
+  </si>
+  <si>
+    <t>joint distribution</t>
+  </si>
+  <si>
+    <t>experimental designs</t>
+  </si>
+  <si>
+    <t>conditional distribution</t>
+  </si>
+  <si>
+    <t>quasi-experimental designs</t>
+  </si>
+  <si>
+    <t>probability trees</t>
+  </si>
+  <si>
+    <t>natural experiment</t>
+  </si>
+  <si>
+    <t>Expected value</t>
+  </si>
+  <si>
+    <t>Monte Carlo Simulations</t>
+  </si>
+  <si>
+    <t>Markov Chain Models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1366,10 +1540,16 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF27515E"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1938,7 +2118,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2048,13 +2228,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2076,90 +2258,92 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2449,10 +2633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124:D124"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2472,11 +2656,11 @@
         <v>143</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D1" s="54"/>
       <c r="G1" s="53" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H1" s="53"/>
     </row>
@@ -2496,7 +2680,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -2511,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -2525,7 +2709,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="37" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2539,7 +2723,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="37" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2553,7 +2737,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -2567,7 +2751,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -3500,9 +3684,413 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="39"/>
-      <c r="B124" s="39"/>
+      <c r="B124" s="39" t="s">
+        <v>412</v>
+      </c>
       <c r="C124" s="39"/>
       <c r="D124" s="39"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="33"/>
+      <c r="B125" s="90" t="s">
+        <v>425</v>
+      </c>
+      <c r="C125" s="33"/>
+      <c r="D125" s="33"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="33"/>
+      <c r="B126" s="90" t="s">
+        <v>427</v>
+      </c>
+      <c r="C126" s="33"/>
+      <c r="D126" s="33"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="33"/>
+      <c r="B127" s="90" t="s">
+        <v>429</v>
+      </c>
+      <c r="C127" s="33"/>
+      <c r="D127" s="33"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="33"/>
+      <c r="B128" s="90" t="s">
+        <v>431</v>
+      </c>
+      <c r="C128" s="33"/>
+      <c r="D128" s="33"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="33"/>
+      <c r="B129" s="90" t="s">
+        <v>432</v>
+      </c>
+      <c r="C129" s="33"/>
+      <c r="D129" s="33"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="33"/>
+      <c r="B130" s="90" t="s">
+        <v>434</v>
+      </c>
+      <c r="C130" s="33"/>
+      <c r="D130" s="33"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="33"/>
+      <c r="B131" s="90" t="s">
+        <v>436</v>
+      </c>
+      <c r="C131" s="33"/>
+      <c r="D131" s="33"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="33"/>
+      <c r="B132" s="90" t="s">
+        <v>439</v>
+      </c>
+      <c r="C132" s="33"/>
+      <c r="D132" s="33"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="33"/>
+      <c r="B133" s="90" t="s">
+        <v>441</v>
+      </c>
+      <c r="C133" s="33"/>
+      <c r="D133" s="33"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="33"/>
+      <c r="B134" s="90" t="s">
+        <v>443</v>
+      </c>
+      <c r="C134" s="33"/>
+      <c r="D134" s="33"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="33"/>
+      <c r="B135" s="90" t="s">
+        <v>445</v>
+      </c>
+      <c r="C135" s="33"/>
+      <c r="D135" s="33"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="33"/>
+      <c r="B136" s="90" t="s">
+        <v>447</v>
+      </c>
+      <c r="C136" s="33"/>
+      <c r="D136" s="33"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" s="33"/>
+      <c r="B137" s="90" t="s">
+        <v>449</v>
+      </c>
+      <c r="C137" s="33"/>
+      <c r="D137" s="33"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="33"/>
+      <c r="B138" s="90" t="s">
+        <v>451</v>
+      </c>
+      <c r="C138" s="33"/>
+      <c r="D138" s="33"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" s="33"/>
+      <c r="B139" s="90" t="s">
+        <v>453</v>
+      </c>
+      <c r="C139" s="33"/>
+      <c r="D139" s="33"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="33"/>
+      <c r="B140" s="90" t="s">
+        <v>455</v>
+      </c>
+      <c r="C140" s="33"/>
+      <c r="D140" s="33"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" s="33"/>
+      <c r="B141" s="90" t="s">
+        <v>458</v>
+      </c>
+      <c r="C141" s="33"/>
+      <c r="D141" s="33"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" s="33"/>
+      <c r="B142" s="90" t="s">
+        <v>460</v>
+      </c>
+      <c r="C142" s="33"/>
+      <c r="D142" s="33"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" s="33"/>
+      <c r="B143" s="90" t="s">
+        <v>462</v>
+      </c>
+      <c r="C143" s="33"/>
+      <c r="D143" s="33"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" s="33"/>
+      <c r="B144" s="90" t="s">
+        <v>464</v>
+      </c>
+      <c r="C144" s="33"/>
+      <c r="D144" s="33"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" s="33"/>
+      <c r="B145" s="90" t="s">
+        <v>466</v>
+      </c>
+      <c r="C145" s="33"/>
+      <c r="D145" s="33"/>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="33"/>
+      <c r="B146" s="90" t="s">
+        <v>468</v>
+      </c>
+      <c r="C146" s="33"/>
+      <c r="D146" s="33"/>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147" s="33"/>
+      <c r="B147" s="90" t="s">
+        <v>470</v>
+      </c>
+      <c r="C147" s="33"/>
+      <c r="D147" s="33"/>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" s="52"/>
+      <c r="B148" s="52" t="s">
+        <v>412</v>
+      </c>
+      <c r="C148" s="52"/>
+      <c r="D148" s="52"/>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="33"/>
+      <c r="B149" s="90" t="s">
+        <v>426</v>
+      </c>
+      <c r="C149" s="33"/>
+      <c r="D149" s="33"/>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="33"/>
+      <c r="B150" s="90" t="s">
+        <v>428</v>
+      </c>
+      <c r="C150" s="33"/>
+      <c r="D150" s="33"/>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="33"/>
+      <c r="B151" s="90" t="s">
+        <v>430</v>
+      </c>
+      <c r="C151" s="33"/>
+      <c r="D151" s="33"/>
+      <c r="H151" s="90"/>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="33"/>
+      <c r="B152" s="90" t="s">
+        <v>433</v>
+      </c>
+      <c r="C152" s="33"/>
+      <c r="D152" s="33"/>
+      <c r="H152" s="90"/>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="33"/>
+      <c r="B153" s="90" t="s">
+        <v>435</v>
+      </c>
+      <c r="C153" s="33"/>
+      <c r="D153" s="33"/>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="33"/>
+      <c r="B154" s="90" t="s">
+        <v>437</v>
+      </c>
+      <c r="C154" s="33"/>
+      <c r="D154" s="33"/>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" s="33"/>
+      <c r="B155" s="90" t="s">
+        <v>438</v>
+      </c>
+      <c r="C155" s="33"/>
+      <c r="D155" s="33"/>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" s="33"/>
+      <c r="B156" s="90" t="s">
+        <v>440</v>
+      </c>
+      <c r="C156" s="33"/>
+      <c r="D156" s="33"/>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" s="33"/>
+      <c r="B157" s="90" t="s">
+        <v>442</v>
+      </c>
+      <c r="C157" s="33"/>
+      <c r="D157" s="33"/>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" s="33"/>
+      <c r="B158" s="90" t="s">
+        <v>444</v>
+      </c>
+      <c r="C158" s="33"/>
+      <c r="D158" s="33"/>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" s="33"/>
+      <c r="B159" s="90" t="s">
+        <v>446</v>
+      </c>
+      <c r="C159" s="33"/>
+      <c r="D159" s="33"/>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" s="33"/>
+      <c r="B160" s="90" t="s">
+        <v>448</v>
+      </c>
+      <c r="C160" s="33"/>
+      <c r="D160" s="33"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="33"/>
+      <c r="B161" s="90" t="s">
+        <v>450</v>
+      </c>
+      <c r="C161" s="33"/>
+      <c r="D161" s="33"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="33"/>
+      <c r="B162" s="90" t="s">
+        <v>452</v>
+      </c>
+      <c r="C162" s="33"/>
+      <c r="D162" s="33"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="33"/>
+      <c r="B163" s="90" t="s">
+        <v>454</v>
+      </c>
+      <c r="C163" s="33"/>
+      <c r="D163" s="33"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="33"/>
+      <c r="B164" s="90" t="s">
+        <v>456</v>
+      </c>
+      <c r="C164" s="33"/>
+      <c r="D164" s="33"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="33"/>
+      <c r="B165" s="90" t="s">
+        <v>457</v>
+      </c>
+      <c r="C165" s="33"/>
+      <c r="D165" s="33"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="33"/>
+      <c r="B166" s="90" t="s">
+        <v>459</v>
+      </c>
+      <c r="C166" s="33"/>
+      <c r="D166" s="33"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="33"/>
+      <c r="B167" s="90" t="s">
+        <v>461</v>
+      </c>
+      <c r="C167" s="33"/>
+      <c r="D167" s="33"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="33"/>
+      <c r="B168" s="90" t="s">
+        <v>463</v>
+      </c>
+      <c r="C168" s="33"/>
+      <c r="D168" s="33"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="33"/>
+      <c r="B169" s="90" t="s">
+        <v>465</v>
+      </c>
+      <c r="C169" s="33"/>
+      <c r="D169" s="33"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="33"/>
+      <c r="B170" s="90" t="s">
+        <v>467</v>
+      </c>
+      <c r="C170" s="33"/>
+      <c r="D170" s="33"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="33"/>
+      <c r="B171" s="90" t="s">
+        <v>469</v>
+      </c>
+      <c r="C171" s="33"/>
+      <c r="D171" s="33"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="33"/>
+      <c r="B172" s="90" t="s">
+        <v>471</v>
+      </c>
+      <c r="C172" s="33"/>
+      <c r="D172" s="33"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="33"/>
+      <c r="B173" s="90" t="s">
+        <v>472</v>
+      </c>
+      <c r="C173" s="33"/>
+      <c r="D173" s="33"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="33"/>
+      <c r="B174" s="90" t="s">
+        <v>473</v>
+      </c>
+      <c r="C174" s="33"/>
+      <c r="D174" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3515,10 +4103,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3532,18 +4120,18 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="41" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -3575,7 +4163,7 @@
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
       <c r="E5" s="55" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F5" s="56"/>
     </row>
@@ -3590,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="46" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3604,12 +4192,12 @@
         <v>1</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="39" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -3618,7 +4206,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="46" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3632,7 +4220,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3651,7 +4239,7 @@
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="57" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F11" s="58"/>
     </row>
@@ -3666,12 +4254,12 @@
         <v>0</v>
       </c>
       <c r="F12" s="44" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="39" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -3680,7 +4268,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="44" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3694,7 +4282,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3708,7 +4296,7 @@
         <v>3</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -3722,7 +4310,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3741,13 +4329,13 @@
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="59" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F18" s="60"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="39" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
@@ -3756,7 +4344,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="48" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3770,7 +4358,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="48" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3784,7 +4372,7 @@
         <v>2</v>
       </c>
       <c r="F21" s="48" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3798,12 +4386,12 @@
         <v>3</v>
       </c>
       <c r="F22" s="48" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -3812,7 +4400,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="48" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3826,7 +4414,7 @@
         <v>5</v>
       </c>
       <c r="F24" s="49" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3871,7 +4459,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
@@ -3911,7 +4499,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="39" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
@@ -3983,7 +4571,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="s">
-        <v>390</v>
+        <v>412</v>
       </c>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
@@ -4031,23 +4619,23 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>305</v>
+        <v>419</v>
       </c>
       <c r="B50" s="33"/>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="52" t="s">
-        <v>411</v>
-      </c>
-      <c r="B51" s="52"/>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
+      <c r="A51" t="s">
+        <v>420</v>
+      </c>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="33"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>306</v>
+        <v>421</v>
       </c>
       <c r="B52" s="33"/>
       <c r="C52" s="33"/>
@@ -4055,91 +4643,130 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>307</v>
+        <v>422</v>
       </c>
       <c r="B53" s="33"/>
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>308</v>
-      </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
+      <c r="A54" s="51" t="s">
+        <v>423</v>
+      </c>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>309</v>
+      <c r="A55" s="90" t="s">
+        <v>305</v>
       </c>
       <c r="B55" s="33"/>
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>310</v>
+      <c r="A56" s="90" t="s">
+        <v>306</v>
       </c>
       <c r="B56" s="33"/>
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>311</v>
+      <c r="A57" s="90" t="s">
+        <v>307</v>
       </c>
       <c r="B57" s="33"/>
       <c r="C57" s="33"/>
       <c r="D57" s="33"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>312</v>
+      <c r="A58" s="90" t="s">
+        <v>308</v>
       </c>
       <c r="B58" s="33"/>
       <c r="C58" s="33"/>
       <c r="D58" s="33"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>313</v>
+      <c r="A59" s="90" t="s">
+        <v>309</v>
       </c>
       <c r="B59" s="33"/>
       <c r="C59" s="33"/>
       <c r="D59" s="33"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="39" t="s">
-        <v>412</v>
-      </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
+      <c r="A60" s="90" t="s">
+        <v>310</v>
+      </c>
+      <c r="B60" s="33"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>413</v>
+      <c r="A61" s="90" t="s">
+        <v>311</v>
       </c>
       <c r="B61" s="33"/>
       <c r="C61" s="33"/>
       <c r="D61" s="33"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>414</v>
+      <c r="A62" s="90" t="s">
+        <v>312</v>
       </c>
       <c r="B62" s="33"/>
       <c r="C62" s="33"/>
       <c r="D62" s="33"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>415</v>
+      <c r="A63" s="90" t="s">
+        <v>409</v>
       </c>
       <c r="B63" s="33"/>
       <c r="C63" s="33"/>
       <c r="D63" s="33"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="90" t="s">
+        <v>410</v>
+      </c>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="90" t="s">
+        <v>411</v>
+      </c>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="39" t="s">
+        <v>424</v>
+      </c>
+      <c r="B66" s="39"/>
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="33"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
+      <c r="D68" s="33"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4153,10 +4780,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4169,166 +4796,166 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="38" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D1" s="53" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B2" s="39"/>
       <c r="D2" s="36">
         <v>0</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B3" s="33"/>
       <c r="D3" s="36">
         <v>1</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B4" s="33"/>
       <c r="D4" s="36">
         <v>2</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B5" s="33"/>
       <c r="D5" s="36">
         <v>3</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B6" s="33"/>
       <c r="D6" s="36">
         <v>4</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B8" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B10" s="33"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B11" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B13" s="33"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="39" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B14" s="39"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B15" s="33"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B16" s="33"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B17" s="33"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="39" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B18" s="39"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B19" s="33"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B20" s="33"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B21" s="33"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B22" s="33"/>
     </row>
@@ -4337,217 +4964,264 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B24" s="33"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B25" s="33"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B26" s="33"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B27" s="33"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="39" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B28" s="39"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B29" s="50"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B30" s="33"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B31" s="33"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B32" s="33"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B33" s="33"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B34" s="33"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B35" s="33"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B36" s="39"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B37" s="33"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B38" s="33"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B39" s="33"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B40" s="33"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B41" s="33"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B42" s="33"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B43" s="39"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B44" s="50"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B45" s="33"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B46" s="33"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B47" s="33"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B48" s="33"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="39" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B49" s="39"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B50" s="33"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B51" s="33"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B52" s="33"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B53" s="33"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B54" s="33"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B55" s="33"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B56" s="33"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B57" s="33"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B58" s="33"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="51"/>
-      <c r="B59" s="51"/>
+      <c r="A59" s="52" t="s">
+        <v>412</v>
+      </c>
+      <c r="B59" s="52"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="89" t="s">
+        <v>413</v>
+      </c>
+      <c r="B60" s="33"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="89" t="s">
+        <v>414</v>
+      </c>
+      <c r="B61" s="33"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="89" t="s">
+        <v>415</v>
+      </c>
+      <c r="B62" s="33"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="89" t="s">
+        <v>416</v>
+      </c>
+      <c r="B63" s="33"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="89" t="s">
+        <v>417</v>
+      </c>
+      <c r="B64" s="33"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="89" t="s">
+        <v>418</v>
+      </c>
+      <c r="B65" s="33"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="52" t="s">
+        <v>423</v>
+      </c>
+      <c r="B66" s="52"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4564,8 +5238,8 @@
   </sheetPr>
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="C17" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A26" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4579,64 +5253,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="79"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="72"/>
     </row>
     <row r="2" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="73" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="82"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="75"/>
     </row>
     <row r="3" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
     </row>
     <row r="4" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="86"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="79"/>
     </row>
     <row r="5" spans="1:6" ht="103" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="80" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="88"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="73"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="83"/>
       <c r="C6" s="8" t="s">
         <v>34</v>
       </c>
@@ -4651,29 +5325,29 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="68"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="63"/>
     </row>
     <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="69"/>
-      <c r="B8" s="74" t="s">
+      <c r="A8" s="65"/>
+      <c r="B8" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="76"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="86"/>
     </row>
     <row r="9" spans="1:6" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="69"/>
+      <c r="A9" s="65"/>
       <c r="B9" s="24" t="s">
         <v>49</v>
       </c>
@@ -4691,7 +5365,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="70"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="15" t="s">
         <v>50</v>
       </c>
@@ -4709,29 +5383,29 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
     </row>
     <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
-      <c r="B12" s="63" t="s">
+      <c r="A12" s="65"/>
+      <c r="B12" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="69"/>
     </row>
     <row r="13" spans="1:6" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
+      <c r="A13" s="65"/>
       <c r="B13" s="24" t="s">
         <v>51</v>
       </c>
@@ -4749,7 +5423,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
+      <c r="A14" s="65"/>
       <c r="B14" s="15" t="s">
         <v>52</v>
       </c>
@@ -4767,29 +5441,29 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="43" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="71" t="s">
+      <c r="A15" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="68"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="63"/>
     </row>
     <row r="16" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="69"/>
-      <c r="B16" s="63" t="s">
+      <c r="A16" s="65"/>
+      <c r="B16" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="65"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="69"/>
     </row>
     <row r="17" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A17" s="69"/>
+      <c r="A17" s="65"/>
       <c r="B17" s="24" t="s">
         <v>53</v>
       </c>
@@ -4807,7 +5481,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="70"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="15" t="s">
         <v>54</v>
       </c>
@@ -4825,29 +5499,29 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="68"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="63"/>
     </row>
     <row r="20" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="69"/>
-      <c r="B20" s="63" t="s">
+      <c r="A20" s="65"/>
+      <c r="B20" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="65"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="69"/>
     </row>
     <row r="21" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A21" s="69"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="24" t="s">
         <v>55</v>
       </c>
@@ -4865,7 +5539,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="69"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="15" t="s">
         <v>56</v>
       </c>
@@ -4883,29 +5557,29 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="68"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="63"/>
     </row>
     <row r="24" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="69"/>
-      <c r="B24" s="63" t="s">
+      <c r="A24" s="65"/>
+      <c r="B24" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="65"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="69"/>
     </row>
     <row r="25" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A25" s="69"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="24" t="s">
         <v>57</v>
       </c>
@@ -4923,7 +5597,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
+      <c r="A26" s="66"/>
       <c r="B26" s="15" t="s">
         <v>58</v>
       </c>
@@ -4941,29 +5615,29 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="68"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="63"/>
     </row>
     <row r="28" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="69"/>
-      <c r="B28" s="63" t="s">
+      <c r="A28" s="65"/>
+      <c r="B28" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="65"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="69"/>
     </row>
     <row r="29" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A29" s="69"/>
+      <c r="A29" s="65"/>
       <c r="B29" s="24" t="s">
         <v>59</v>
       </c>
@@ -4981,7 +5655,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
+      <c r="A30" s="65"/>
       <c r="B30" s="15" t="s">
         <v>60</v>
       </c>
@@ -4999,29 +5673,29 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="68"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="63"/>
     </row>
     <row r="32" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="69"/>
-      <c r="B32" s="63" t="s">
+      <c r="A32" s="65"/>
+      <c r="B32" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="65"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="69"/>
     </row>
     <row r="33" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A33" s="69"/>
+      <c r="A33" s="65"/>
       <c r="B33" s="24" t="s">
         <v>74</v>
       </c>
@@ -5039,7 +5713,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="70"/>
+      <c r="A34" s="66"/>
       <c r="B34" s="15" t="s">
         <v>78</v>
       </c>
@@ -5057,29 +5731,29 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="66" t="s">
+      <c r="B35" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="68"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="63"/>
     </row>
     <row r="36" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="69"/>
-      <c r="B36" s="63" t="s">
+      <c r="A36" s="65"/>
+      <c r="B36" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="65"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="69"/>
     </row>
     <row r="37" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A37" s="69"/>
+      <c r="A37" s="65"/>
       <c r="B37" s="24" t="s">
         <v>61</v>
       </c>
@@ -5097,7 +5771,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="65" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="69"/>
+      <c r="A38" s="65"/>
       <c r="B38" s="15" t="s">
         <v>62</v>
       </c>
@@ -5115,29 +5789,29 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="71" t="s">
+      <c r="A39" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="66" t="s">
+      <c r="B39" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="68"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="63"/>
     </row>
     <row r="40" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="69"/>
-      <c r="B40" s="63" t="s">
+      <c r="A40" s="65"/>
+      <c r="B40" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="65"/>
+      <c r="C40" s="68"/>
+      <c r="D40" s="68"/>
+      <c r="E40" s="68"/>
+      <c r="F40" s="69"/>
     </row>
     <row r="41" spans="1:6" ht="77" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="69"/>
+      <c r="A41" s="65"/>
       <c r="B41" s="24" t="s">
         <v>63</v>
       </c>
@@ -5155,7 +5829,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="70"/>
+      <c r="A42" s="66"/>
       <c r="B42" s="15" t="s">
         <v>95</v>
       </c>
@@ -5173,29 +5847,29 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="69" t="s">
+      <c r="A43" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="68"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="63"/>
     </row>
     <row r="44" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="69"/>
-      <c r="B44" s="63" t="s">
+      <c r="A44" s="65"/>
+      <c r="B44" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="64"/>
-      <c r="D44" s="64"/>
-      <c r="E44" s="64"/>
-      <c r="F44" s="65"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="69"/>
     </row>
     <row r="45" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A45" s="69"/>
+      <c r="A45" s="65"/>
       <c r="B45" s="24" t="s">
         <v>64</v>
       </c>
@@ -5213,7 +5887,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="81" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="70"/>
+      <c r="A46" s="66"/>
       <c r="B46" s="15" t="s">
         <v>65</v>
       </c>
@@ -5231,8 +5905,8 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="61"/>
-      <c r="B47" s="62"/>
+      <c r="A47" s="87"/>
+      <c r="B47" s="88"/>
       <c r="C47" s="20" t="s">
         <v>0</v>
       </c>
@@ -5266,19 +5940,16 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="A39:A42"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B12:F12"/>
@@ -5293,16 +5964,19 @@
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B20:F20"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A38"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B27:F27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>